<commit_message>
Added Course Materials - Day 16
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Track 2 - TOC.xlsx
+++ b/Java Apps @ DXC - Track 2 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -2108,10 +2108,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -2266,13 +2266,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2280,7 +2273,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2291,6 +2299,14 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2311,25 +2327,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2364,6 +2365,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2380,22 +2388,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2455,6 +2455,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2473,7 +2509,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2485,31 +2521,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2527,7 +2539,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2539,37 +2605,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2581,13 +2623,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2599,43 +2635,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2732,8 +2732,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2753,15 +2753,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2773,6 +2764,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2812,165 +2818,159 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="31" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="31" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3614,7 +3614,7 @@
   <sheetPr/>
   <dimension ref="A1:D331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
@@ -6001,10 +6001,10 @@
   <sheetPr/>
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Added Hands On Demos - Day 21
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Track 2 - TOC.xlsx
+++ b/Java Apps @ DXC - Track 2 - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="657">
   <si>
     <t>Track 2</t>
   </si>
@@ -1766,7 +1766,7 @@
 Validations</t>
   </si>
   <si>
-    <t>15. Introduction to TemplateDriven Forms</t>
+    <t>2. Introduction to TemplateDriven Forms</t>
   </si>
   <si>
     <t>1. Module Overview</t>
@@ -1781,7 +1781,7 @@
     <t>5. Validations</t>
   </si>
   <si>
-    <t>16. Template-driven vs. Reactive Forms</t>
+    <t>3. Template-driven vs. Reactive Forms</t>
   </si>
   <si>
     <t>2. Form Building Blocks</t>
@@ -1807,7 +1807,7 @@
 Custom Validations</t>
   </si>
   <si>
-    <t>17. Building a Reactive Form</t>
+    <t>4. Building a Reactive Form</t>
   </si>
   <si>
     <t>2. The Component Class</t>
@@ -1844,7 +1844,7 @@
 Consuming REST end Points using HttpClient                                A sample CRUD application</t>
   </si>
   <si>
-    <t>18. Validation</t>
+    <t>5. Validation</t>
   </si>
   <si>
     <t>2. Setting Built-in Validation Rules</t>
@@ -1865,7 +1865,7 @@
     <t>7. Cross-Field Validation-Custom Validator</t>
   </si>
   <si>
-    <t>19. Create, Read, Update, and Delete (CRUD) Using HTTP</t>
+    <t>6. Create, Read, Update, and Delete (CRUD) Using HTTP</t>
   </si>
   <si>
     <t>2. Data Access Service</t>
@@ -1910,7 +1910,7 @@
     <t>Bootstrap Integration</t>
   </si>
   <si>
-    <t>20. Bootstrap Integration with Angular</t>
+    <t>7. Bootstrap Integration with Angular</t>
   </si>
   <si>
     <t>1. Getting Started with ng-bootstrap</t>
@@ -1938,7 +1938,7 @@
 </t>
   </si>
   <si>
-    <t>21. Create Multiple Angular Apps in One Project</t>
+    <t>8. Create Multiple Angular Apps in One Project</t>
   </si>
   <si>
     <t>1. Advantages</t>
@@ -2114,10 +2114,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -2272,7 +2272,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2280,7 +2280,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2295,7 +2309,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2308,32 +2337,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2349,43 +2363,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2401,15 +2379,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2461,49 +2461,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2533,7 +2503,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2545,19 +2599,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2569,7 +2623,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2581,67 +2635,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2735,17 +2735,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2765,11 +2776,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2791,51 +2832,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2853,130 +2853,130 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6016,7 +6016,7 @@
   <sheetPr/>
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
@@ -7189,12 +7189,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D219"/>
+  <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D114" sqref="D114"/>
+      <selection pane="bottomLeft" activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -8201,549 +8201,563 @@
     </row>
     <row r="138" ht="18.75" spans="1:3">
       <c r="A138" s="16"/>
-      <c r="B138" s="17"/>
+      <c r="B138" s="6"/>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" ht="15" spans="1:3">
+    <row r="139" ht="18.75" spans="1:3">
       <c r="A139" s="16" t="s">
         <v>543</v>
       </c>
-      <c r="B139" s="6" t="s">
-        <v>544</v>
+      <c r="B139" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="140" ht="15" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" ht="18.75" spans="1:3">
       <c r="A140" s="16"/>
-      <c r="B140" s="6"/>
-      <c r="C140" s="4" t="s">
-        <v>546</v>
-      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="4"/>
     </row>
     <row r="141" ht="15" spans="1:3">
       <c r="A141" s="16"/>
-      <c r="B141" s="6"/>
+      <c r="B141" s="6" t="s">
+        <v>544</v>
+      </c>
       <c r="C141" s="4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="142" ht="15" spans="1:3">
       <c r="A142" s="16"/>
       <c r="B142" s="6"/>
       <c r="C142" s="4" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="143" ht="18" spans="1:3">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="143" ht="15" spans="1:3">
       <c r="A143" s="16"/>
-      <c r="B143" s="17"/>
-      <c r="C143" s="4"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="4" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="144" ht="15" spans="1:3">
       <c r="A144" s="16"/>
-      <c r="B144" s="6" t="s">
-        <v>549</v>
-      </c>
+      <c r="B144" s="6"/>
       <c r="C144" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="145" ht="15" spans="1:3">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="145" ht="18" spans="1:3">
       <c r="A145" s="16"/>
-      <c r="B145" s="6"/>
-      <c r="C145" s="4" t="s">
-        <v>550</v>
-      </c>
+      <c r="B145" s="17"/>
+      <c r="C145" s="4"/>
     </row>
     <row r="146" ht="15" spans="1:3">
       <c r="A146" s="16"/>
-      <c r="B146" s="6"/>
+      <c r="B146" s="6" t="s">
+        <v>549</v>
+      </c>
       <c r="C146" s="4" t="s">
-        <v>551</v>
+        <v>26</v>
       </c>
     </row>
     <row r="147" ht="15" spans="1:3">
       <c r="A147" s="16"/>
       <c r="B147" s="6"/>
       <c r="C147" s="4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="148" ht="15" spans="1:3">
       <c r="A148" s="16"/>
       <c r="B148" s="6"/>
       <c r="C148" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="149" ht="15" spans="1:3">
       <c r="A149" s="16"/>
       <c r="B149" s="6"/>
       <c r="C149" s="4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="150" ht="15" spans="1:3">
       <c r="A150" s="16"/>
       <c r="B150" s="6"/>
       <c r="C150" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="151" ht="15" spans="1:3">
       <c r="A151" s="16"/>
       <c r="B151" s="6"/>
       <c r="C151" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="152" ht="15" spans="1:3">
+      <c r="A152" s="16"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="153" ht="15" spans="1:3">
+      <c r="A153" s="16"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="152" ht="15" spans="2:3">
-      <c r="B152" s="21"/>
-      <c r="C152" s="4"/>
-    </row>
-    <row r="153" ht="15" spans="1:3">
-      <c r="A153" s="16" t="s">
+    <row r="154" ht="15" spans="2:3">
+      <c r="B154" s="21"/>
+      <c r="C154" s="4"/>
+    </row>
+    <row r="155" ht="15" spans="1:3">
+      <c r="A155" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="B153" s="6" t="s">
+      <c r="B155" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="C153" s="4" t="s">
+      <c r="C155" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="154" ht="15" spans="1:3">
-      <c r="A154" s="16"/>
-      <c r="B154" s="6"/>
-      <c r="C154" s="4" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="155" ht="15" spans="1:3">
-      <c r="A155" s="16"/>
-      <c r="B155" s="6"/>
-      <c r="C155" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="156" ht="15" spans="1:3">
       <c r="A156" s="16"/>
       <c r="B156" s="6"/>
       <c r="C156" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="157" ht="15" spans="1:3">
       <c r="A157" s="16"/>
       <c r="B157" s="6"/>
       <c r="C157" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="158" ht="15" spans="1:3">
       <c r="A158" s="16"/>
       <c r="B158" s="6"/>
       <c r="C158" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="159" ht="15" spans="1:3">
       <c r="A159" s="16"/>
       <c r="B159" s="6"/>
       <c r="C159" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="160" ht="15" spans="1:3">
       <c r="A160" s="16"/>
       <c r="B160" s="6"/>
       <c r="C160" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="161" ht="15" spans="1:3">
       <c r="A161" s="16"/>
       <c r="B161" s="6"/>
       <c r="C161" s="4" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="162" ht="18.75" spans="1:3">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="162" ht="15" spans="1:3">
       <c r="A162" s="16"/>
-      <c r="B162" s="17"/>
-      <c r="C162" s="4"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="4" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="163" ht="15" spans="1:3">
       <c r="A163" s="16"/>
-      <c r="B163" s="9" t="s">
+      <c r="B163" s="6"/>
+      <c r="C163" s="4" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="164" ht="18.75" spans="1:3">
+      <c r="A164" s="16"/>
+      <c r="B164" s="17"/>
+      <c r="C164" s="4"/>
+    </row>
+    <row r="165" ht="15" spans="1:3">
+      <c r="A165" s="16"/>
+      <c r="B165" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C163" s="10" t="s">
+      <c r="C165" s="10" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="164" ht="15" spans="1:3">
-      <c r="A164" s="16"/>
-      <c r="B164" s="9"/>
-      <c r="C164" s="4" t="s">
+    <row r="166" ht="15" spans="1:3">
+      <c r="A166" s="16"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="4" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="165" ht="13" customHeight="1" spans="1:3">
-      <c r="A165" s="22"/>
-      <c r="B165" s="22"/>
-      <c r="C165" s="22"/>
-    </row>
-    <row r="166" ht="24.75" spans="1:3">
-      <c r="A166" s="2" t="s">
+    <row r="167" ht="13" customHeight="1" spans="1:3">
+      <c r="A167" s="22"/>
+      <c r="B167" s="22"/>
+      <c r="C167" s="22"/>
+    </row>
+    <row r="168" ht="24.75" spans="1:3">
+      <c r="A168" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
-    </row>
-    <row r="167" ht="15" spans="1:3">
-      <c r="A167" s="16" t="s">
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
+    </row>
+    <row r="169" ht="15" spans="1:3">
+      <c r="A169" s="16" t="s">
         <v>568</v>
       </c>
-      <c r="B167" s="6" t="s">
+      <c r="B169" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="C169" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="168" ht="15" spans="1:3">
-      <c r="A168" s="16"/>
-      <c r="B168" s="6"/>
-      <c r="C168" s="4" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="169" ht="15" spans="1:3">
-      <c r="A169" s="16"/>
-      <c r="B169" s="6"/>
-      <c r="C169" s="4" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="170" ht="15" spans="1:3">
       <c r="A170" s="16"/>
       <c r="B170" s="6"/>
       <c r="C170" s="4" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="171" ht="15" spans="1:3">
       <c r="A171" s="16"/>
       <c r="B171" s="6"/>
       <c r="C171" s="4" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="172" ht="15" spans="1:3">
       <c r="A172" s="16"/>
       <c r="B172" s="6"/>
       <c r="C172" s="4" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="173" ht="15" spans="1:3">
       <c r="A173" s="16"/>
       <c r="B173" s="6"/>
       <c r="C173" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="174" ht="15" spans="1:3">
       <c r="A174" s="16"/>
       <c r="B174" s="6"/>
       <c r="C174" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="175" ht="15" spans="1:3">
+      <c r="A175" s="16"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="176" ht="15" spans="1:3">
+      <c r="A176" s="16"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="4" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="16"/>
-      <c r="C175" s="21"/>
-    </row>
-    <row r="176" ht="23" customHeight="1" spans="1:3">
-      <c r="A176" s="16"/>
-      <c r="B176" s="6" t="s">
+    <row r="177" spans="1:3">
+      <c r="A177" s="16"/>
+      <c r="C177" s="21"/>
+    </row>
+    <row r="178" ht="23" customHeight="1" spans="1:3">
+      <c r="A178" s="16"/>
+      <c r="B178" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C178" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="177" ht="15" spans="1:3">
-      <c r="A177" s="16"/>
-      <c r="B177" s="6"/>
-      <c r="C177" s="4" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="178" ht="15" spans="1:3">
-      <c r="A178" s="16"/>
-      <c r="B178" s="6"/>
-      <c r="C178" s="4" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="179" ht="15" spans="1:3">
       <c r="A179" s="16"/>
       <c r="B179" s="6"/>
       <c r="C179" s="4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="180" ht="15" spans="1:3">
       <c r="A180" s="16"/>
       <c r="B180" s="6"/>
       <c r="C180" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="181" ht="15" spans="1:3">
       <c r="A181" s="16"/>
       <c r="B181" s="6"/>
       <c r="C181" s="4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="182" ht="15" spans="1:3">
       <c r="A182" s="16"/>
       <c r="B182" s="6"/>
       <c r="C182" s="4" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="183" ht="15" spans="1:3">
       <c r="A183" s="16"/>
       <c r="B183" s="6"/>
       <c r="C183" s="4" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="184" ht="15" spans="1:3">
       <c r="A184" s="16"/>
       <c r="B184" s="6"/>
       <c r="C184" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="185" ht="15" spans="1:3">
       <c r="A185" s="16"/>
       <c r="B185" s="6"/>
       <c r="C185" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="186" ht="15" spans="1:3">
       <c r="A186" s="16"/>
       <c r="B186" s="6"/>
       <c r="C186" s="4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="187" ht="15" spans="1:3">
       <c r="A187" s="16"/>
       <c r="B187" s="6"/>
       <c r="C187" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="188" ht="15" spans="1:3">
       <c r="A188" s="16"/>
       <c r="B188" s="6"/>
       <c r="C188" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="189" ht="15" spans="1:3">
       <c r="A189" s="16"/>
       <c r="B189" s="6"/>
       <c r="C189" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="190" ht="15" spans="1:3">
+      <c r="A190" s="16"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="191" ht="15" spans="1:3">
+      <c r="A191" s="16"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="4" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="190" ht="15" spans="3:3">
-      <c r="C190" s="4"/>
-    </row>
-    <row r="191" ht="15" spans="1:3">
-      <c r="A191" s="16" t="s">
+    <row r="192" ht="15" spans="3:3">
+      <c r="C192" s="4"/>
+    </row>
+    <row r="193" ht="15" spans="1:3">
+      <c r="A193" s="16" t="s">
         <v>590</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="B193" s="6" t="s">
         <v>591</v>
       </c>
-      <c r="C191" s="4" t="s">
+      <c r="C193" s="4" t="s">
         <v>592</v>
-      </c>
-    </row>
-    <row r="192" ht="15" spans="1:3">
-      <c r="A192" s="16"/>
-      <c r="B192" s="6"/>
-      <c r="C192" s="4" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="193" ht="15" spans="1:3">
-      <c r="A193" s="16"/>
-      <c r="B193" s="6"/>
-      <c r="C193" s="4" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="194" ht="15" spans="1:3">
       <c r="A194" s="16"/>
       <c r="B194" s="6"/>
       <c r="C194" s="4" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="195" ht="15" spans="1:3">
       <c r="A195" s="16"/>
       <c r="B195" s="6"/>
       <c r="C195" s="4" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="196" ht="15" spans="1:3">
       <c r="A196" s="16"/>
       <c r="B196" s="6"/>
       <c r="C196" s="4" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="197" ht="15" spans="1:3">
       <c r="A197" s="16"/>
       <c r="B197" s="6"/>
       <c r="C197" s="4" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="198" ht="15" spans="1:3">
+      <c r="A198" s="16"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="199" ht="15" spans="1:3">
+      <c r="A199" s="16"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="4" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="198" ht="15" spans="3:3">
-      <c r="C198" s="4"/>
-    </row>
-    <row r="199" ht="15" spans="1:3">
-      <c r="A199" s="16" t="s">
+    <row r="200" ht="15" spans="3:3">
+      <c r="C200" s="4"/>
+    </row>
+    <row r="201" ht="15" spans="1:3">
+      <c r="A201" s="16" t="s">
         <v>599</v>
       </c>
-      <c r="B199" s="6" t="s">
+      <c r="B201" s="6" t="s">
         <v>600</v>
       </c>
-      <c r="C199" s="4" t="s">
+      <c r="C201" s="4" t="s">
         <v>601</v>
-      </c>
-    </row>
-    <row r="200" ht="15" spans="1:3">
-      <c r="A200" s="16"/>
-      <c r="B200" s="6"/>
-      <c r="C200" s="4" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="201" ht="15" spans="1:3">
-      <c r="A201" s="16"/>
-      <c r="B201" s="6"/>
-      <c r="C201" s="4" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="202" ht="15" spans="1:3">
       <c r="A202" s="16"/>
       <c r="B202" s="6"/>
       <c r="C202" s="4" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="203" ht="15" spans="1:3">
       <c r="A203" s="16"/>
       <c r="B203" s="6"/>
       <c r="C203" s="4" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="204" ht="15" spans="1:3">
       <c r="A204" s="16"/>
       <c r="B204" s="6"/>
       <c r="C204" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="205" ht="15" spans="1:3">
       <c r="A205" s="16"/>
       <c r="B205" s="6"/>
       <c r="C205" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="206" ht="15" spans="1:3">
       <c r="A206" s="16"/>
       <c r="B206" s="6"/>
       <c r="C206" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="207" ht="15" spans="1:3">
       <c r="A207" s="16"/>
       <c r="B207" s="6"/>
       <c r="C207" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="208" ht="15" spans="1:3">
       <c r="A208" s="16"/>
       <c r="B208" s="6"/>
       <c r="C208" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="209" ht="15" spans="1:3">
       <c r="A209" s="16"/>
       <c r="B209" s="6"/>
       <c r="C209" s="4" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="210" ht="15" spans="3:3">
-      <c r="C210" s="4"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="210" ht="15" spans="1:3">
+      <c r="A210" s="16"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="4" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="211" ht="15" spans="1:3">
       <c r="A211" s="16"/>
-      <c r="B211" s="9" t="s">
+      <c r="B211" s="6"/>
+      <c r="C211" s="4" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="212" ht="15" spans="3:3">
+      <c r="C212" s="4"/>
+    </row>
+    <row r="213" ht="15" spans="1:3">
+      <c r="A213" s="16"/>
+      <c r="B213" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C211" s="10" t="s">
+      <c r="C213" s="10" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="212" ht="15" spans="1:3">
-      <c r="A212" s="16"/>
-      <c r="B212" s="9"/>
-      <c r="C212" s="4" t="s">
+    <row r="214" ht="15" spans="1:3">
+      <c r="A214" s="16"/>
+      <c r="B214" s="9"/>
+      <c r="C214" s="4" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="213" ht="11" customHeight="1" spans="1:3">
-      <c r="A213" s="22"/>
-      <c r="B213" s="22"/>
-      <c r="C213" s="22"/>
-    </row>
-    <row r="218" ht="18.75" spans="1:2">
-      <c r="A218" s="23" t="s">
+    <row r="215" ht="11" customHeight="1" spans="1:3">
+      <c r="A215" s="22"/>
+      <c r="B215" s="22"/>
+      <c r="C215" s="22"/>
+    </row>
+    <row r="220" ht="18.75" spans="1:2">
+      <c r="A220" s="23" t="s">
         <v>614</v>
       </c>
-      <c r="B218" s="14">
+      <c r="B220" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="219" ht="18.75" spans="1:2">
-      <c r="A219" s="23" t="s">
+    <row r="221" ht="18.75" spans="1:2">
+      <c r="A221" s="23" t="s">
         <v>615</v>
       </c>
-      <c r="B219" s="14">
+      <c r="B221" s="14">
         <v>32</v>
       </c>
     </row>
@@ -8753,9 +8767,9 @@
     <mergeCell ref="A52:C52"/>
     <mergeCell ref="A74:C74"/>
     <mergeCell ref="A115:C115"/>
-    <mergeCell ref="A165:C165"/>
-    <mergeCell ref="A166:C166"/>
-    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A167:C167"/>
+    <mergeCell ref="A168:C168"/>
+    <mergeCell ref="A215:C215"/>
     <mergeCell ref="A3:A19"/>
     <mergeCell ref="A21:A30"/>
     <mergeCell ref="A32:A39"/>
@@ -8770,13 +8784,13 @@
     <mergeCell ref="A112:A113"/>
     <mergeCell ref="A116:A129"/>
     <mergeCell ref="A131:A137"/>
-    <mergeCell ref="A139:A151"/>
-    <mergeCell ref="A153:A161"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="A167:A189"/>
-    <mergeCell ref="A191:A197"/>
-    <mergeCell ref="A199:A209"/>
-    <mergeCell ref="A211:A212"/>
+    <mergeCell ref="A139:A153"/>
+    <mergeCell ref="A155:A163"/>
+    <mergeCell ref="A165:A166"/>
+    <mergeCell ref="A169:A191"/>
+    <mergeCell ref="A193:A199"/>
+    <mergeCell ref="A201:A211"/>
+    <mergeCell ref="A213:A214"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B11:B19"/>
     <mergeCell ref="B21:B30"/>
@@ -8792,15 +8806,15 @@
     <mergeCell ref="B112:B113"/>
     <mergeCell ref="B116:B129"/>
     <mergeCell ref="B131:B137"/>
-    <mergeCell ref="B139:B142"/>
-    <mergeCell ref="B144:B151"/>
-    <mergeCell ref="B153:B161"/>
-    <mergeCell ref="B163:B164"/>
-    <mergeCell ref="B167:B174"/>
-    <mergeCell ref="B176:B189"/>
-    <mergeCell ref="B191:B197"/>
-    <mergeCell ref="B199:B209"/>
-    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="B141:B144"/>
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="B155:B163"/>
+    <mergeCell ref="B165:B166"/>
+    <mergeCell ref="B169:B176"/>
+    <mergeCell ref="B178:B191"/>
+    <mergeCell ref="B193:B199"/>
+    <mergeCell ref="B201:B211"/>
+    <mergeCell ref="B213:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -8813,7 +8827,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>

</xml_diff>